<commit_message>
Dodan opis k projektu
</commit_message>
<xml_diff>
--- a/podatki/Povprecje_pridelkov_slovenija.xlsx
+++ b/podatki/Povprecje_pridelkov_slovenija.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakab\Desktop\R-Projekt-Naloga\APPR-2020-21\podatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EB9965-4856-4509-8978-BA6878A0E837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DCA206-120F-46B1-A457-F0CD55F46D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31995" yWindow="2085" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33930" yWindow="2160" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1502410S" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>2010</t>
   </si>
@@ -52,9 +52,6 @@
     <t>2019</t>
   </si>
   <si>
-    <t>Pšenica in pira</t>
-  </si>
-  <si>
     <t>Ječmen</t>
   </si>
   <si>
@@ -64,61 +61,61 @@
     <t>Oves</t>
   </si>
   <si>
-    <t>Rž in soržica</t>
-  </si>
-  <si>
-    <t>Koruza za zrnje</t>
-  </si>
-  <si>
-    <t>Silažna koruza</t>
-  </si>
-  <si>
     <t>Krompir</t>
   </si>
   <si>
     <t>Buče za olje</t>
   </si>
   <si>
-    <t>Oljna ogrščica in repica</t>
-  </si>
-  <si>
     <t>Hmelj</t>
   </si>
   <si>
-    <t>Trave (1 do 5 let)</t>
-  </si>
-  <si>
-    <t>Travno deteljne mešanice (1 do 5 let)</t>
-  </si>
-  <si>
-    <t>Deteljno travne mešanice (1 do 5 let)</t>
-  </si>
-  <si>
     <t>Detelja</t>
   </si>
   <si>
     <t>Lucerna</t>
   </si>
   <si>
-    <t>Trajni travniki in pašniki, vključno s skupnimi travniki in pašniki</t>
-  </si>
-  <si>
-    <t>Belo zelje</t>
-  </si>
-  <si>
     <t>Grozdje</t>
   </si>
   <si>
-    <t>Jabolka v intenzivnih sadovnjakih</t>
-  </si>
-  <si>
     <t>Oljke</t>
   </si>
   <si>
-    <t>Breskve in nektarine v intenzivnih sadovnjakih</t>
-  </si>
-  <si>
-    <t>Povprečni pridelek (t/ha) pomembnejših kmetijskih kultur po: KMETIJSKE KULTURE, LETO , v SLOVENIJI</t>
+    <t>pridelek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pšenica </t>
+  </si>
+  <si>
+    <t>Riž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koruza </t>
+  </si>
+  <si>
+    <t>Silažna</t>
+  </si>
+  <si>
+    <t>Repica</t>
+  </si>
+  <si>
+    <t>Trave</t>
+  </si>
+  <si>
+    <t>Deteljne</t>
+  </si>
+  <si>
+    <t>Trajni travniki</t>
+  </si>
+  <si>
+    <t>Zelje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jabolka </t>
+  </si>
+  <si>
+    <t>Breskve</t>
   </si>
 </sst>
 </file>
@@ -480,9 +477,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -492,7 +491,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -527,7 +526,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3">
         <v>4.8</v>
@@ -562,7 +561,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>4.3</v>
@@ -597,7 +596,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -632,7 +631,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>2.9</v>
@@ -667,7 +666,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>3.4</v>
@@ -702,7 +701,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
         <v>8.5</v>
@@ -737,7 +736,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>44.1</v>
@@ -772,7 +771,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>24.5</v>
@@ -807,7 +806,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>0.6</v>
@@ -842,7 +841,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>2.9</v>
@@ -877,7 +876,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>1.4</v>
@@ -912,7 +911,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>7.3</v>
@@ -947,7 +946,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3">
         <v>7.5</v>
@@ -982,10 +981,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="C15" s="3">
         <v>7.5</v>
@@ -994,312 +993,277 @@
         <v>5.6</v>
       </c>
       <c r="E15" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="F15" s="3">
-        <v>7.6</v>
+        <v>7</v>
       </c>
       <c r="G15" s="3">
-        <v>7.7</v>
+        <v>7.1</v>
       </c>
       <c r="H15" s="3">
-        <v>7.8</v>
+        <v>7.3</v>
       </c>
       <c r="I15" s="3">
-        <v>6</v>
+        <v>5.8</v>
       </c>
       <c r="J15" s="3">
-        <v>7.7</v>
+        <v>6.9</v>
       </c>
       <c r="K15" s="3">
-        <v>7.6</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
       <c r="C16" s="3">
-        <v>7.5</v>
+        <v>7.7</v>
       </c>
       <c r="D16" s="3">
-        <v>5.6</v>
+        <v>6.4</v>
       </c>
       <c r="E16" s="3">
-        <v>5.2</v>
+        <v>6.1</v>
       </c>
       <c r="F16" s="3">
-        <v>7</v>
+        <v>8.1</v>
       </c>
       <c r="G16" s="3">
-        <v>7.1</v>
+        <v>8</v>
       </c>
       <c r="H16" s="3">
-        <v>7.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I16" s="3">
-        <v>5.8</v>
+        <v>6.7</v>
       </c>
       <c r="J16" s="3">
-        <v>6.9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="K16" s="3">
-        <v>6.8</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3">
-        <v>8.1</v>
+        <v>5.7</v>
       </c>
       <c r="C17" s="3">
-        <v>7.7</v>
+        <v>5.5</v>
       </c>
       <c r="D17" s="3">
-        <v>6.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E17" s="3">
-        <v>6.1</v>
+        <v>4.2</v>
       </c>
       <c r="F17" s="3">
-        <v>8.1</v>
+        <v>5.7</v>
       </c>
       <c r="G17" s="3">
-        <v>8</v>
+        <v>5.9</v>
       </c>
       <c r="H17" s="3">
-        <v>8.3000000000000007</v>
+        <v>6</v>
       </c>
       <c r="I17" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="J17" s="3">
-        <v>8.3000000000000007</v>
+        <v>5.8</v>
       </c>
       <c r="K17" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3">
-        <v>5.7</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3">
-        <v>5.5</v>
+        <v>35.9</v>
       </c>
       <c r="D18" s="3">
-        <v>4.5999999999999996</v>
+        <v>28.4</v>
       </c>
       <c r="E18" s="3">
-        <v>4.2</v>
+        <v>25.6</v>
       </c>
       <c r="F18" s="3">
-        <v>5.7</v>
+        <v>32</v>
       </c>
       <c r="G18" s="3">
-        <v>5.9</v>
+        <v>34.4</v>
       </c>
       <c r="H18" s="3">
-        <v>6</v>
+        <v>35.1</v>
       </c>
       <c r="I18" s="3">
-        <v>4.5</v>
+        <v>31.9</v>
       </c>
       <c r="J18" s="3">
-        <v>5.8</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="K18" s="3">
-        <v>5.8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>35</v>
+        <v>6.6</v>
       </c>
       <c r="C19" s="3">
-        <v>35.9</v>
+        <v>7.4</v>
       </c>
       <c r="D19" s="3">
-        <v>28.4</v>
+        <v>5.6</v>
       </c>
       <c r="E19" s="3">
-        <v>25.6</v>
+        <v>6.2</v>
       </c>
       <c r="F19" s="3">
-        <v>32</v>
+        <v>5.9</v>
       </c>
       <c r="G19" s="3">
-        <v>34.4</v>
+        <v>7.5</v>
       </c>
       <c r="H19" s="3">
-        <v>35.1</v>
+        <v>6</v>
       </c>
       <c r="I19" s="3">
-        <v>31.9</v>
+        <v>5.6</v>
       </c>
       <c r="J19" s="3">
-        <v>34.799999999999997</v>
+        <v>8.1</v>
       </c>
       <c r="K19" s="3">
-        <v>34</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3">
         <v>28</v>
       </c>
-      <c r="B20" s="3">
-        <v>6.6</v>
-      </c>
       <c r="C20" s="3">
-        <v>7.4</v>
+        <v>29.7</v>
       </c>
       <c r="D20" s="3">
-        <v>5.6</v>
+        <v>20.5</v>
       </c>
       <c r="E20" s="3">
-        <v>6.2</v>
+        <v>26.3</v>
       </c>
       <c r="F20" s="3">
-        <v>5.9</v>
+        <v>27.9</v>
       </c>
       <c r="G20" s="3">
-        <v>7.5</v>
+        <v>34</v>
       </c>
       <c r="H20" s="3">
-        <v>6</v>
+        <v>17.7</v>
       </c>
       <c r="I20" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="J20" s="3">
-        <v>8.1</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="K20" s="3">
-        <v>6.8</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>28</v>
+        <v>2.1</v>
       </c>
       <c r="C21" s="3">
-        <v>29.7</v>
+        <v>1.9</v>
       </c>
       <c r="D21" s="3">
-        <v>20.5</v>
+        <v>0.8</v>
       </c>
       <c r="E21" s="3">
-        <v>26.3</v>
+        <v>1.6</v>
       </c>
       <c r="F21" s="3">
-        <v>27.9</v>
+        <v>0.8</v>
       </c>
       <c r="G21" s="3">
-        <v>34</v>
+        <v>1.5</v>
       </c>
       <c r="H21" s="3">
-        <v>17.7</v>
+        <v>1.4</v>
       </c>
       <c r="I21" s="3">
-        <v>5.8</v>
+        <v>1.4</v>
       </c>
       <c r="J21" s="3">
-        <v>37.200000000000003</v>
+        <v>3</v>
       </c>
       <c r="K21" s="3">
-        <v>23.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3">
-        <v>2.1</v>
+        <v>15.7</v>
       </c>
       <c r="C22" s="3">
-        <v>1.9</v>
+        <v>16.3</v>
       </c>
       <c r="D22" s="3">
-        <v>0.8</v>
+        <v>13.6</v>
       </c>
       <c r="E22" s="3">
-        <v>1.6</v>
+        <v>14.2</v>
       </c>
       <c r="F22" s="3">
-        <v>0.8</v>
+        <v>11.7</v>
       </c>
       <c r="G22" s="3">
-        <v>1.5</v>
+        <v>17.5</v>
       </c>
       <c r="H22" s="3">
-        <v>1.4</v>
+        <v>15.7</v>
       </c>
       <c r="I22" s="3">
-        <v>1.4</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J22" s="3">
-        <v>3</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="K22" s="3">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="3">
-        <v>15.7</v>
-      </c>
-      <c r="C23" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="D23" s="3">
-        <v>13.6</v>
-      </c>
-      <c r="E23" s="3">
-        <v>14.2</v>
-      </c>
-      <c r="F23" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="G23" s="3">
-        <v>17.5</v>
-      </c>
-      <c r="H23" s="3">
-        <v>15.7</v>
-      </c>
-      <c r="I23" s="3">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="J23" s="3">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="K23" s="3">
         <v>15.1</v>
       </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>